<commit_message>
Complementação da lista com brainstorm
</commit_message>
<xml_diff>
--- a/PastaDocsRequisitos/2SIR-ListaPesquisa.xlsx
+++ b/PastaDocsRequisitos/2SIR-ListaPesquisa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonpflocal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{493AFFA2-418E-44CF-8EEC-2822F5EB7756}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D651E50A-B76E-402F-B4F8-1FA8E2C9988E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" xr2:uid="{0891ED88-779E-4904-AB47-DA324D9A5ACC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8388" xr2:uid="{0891ED88-779E-4904-AB47-DA324D9A5ACC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Requisitos do sistema de gestão de estacionamento</t>
   </si>
@@ -109,16 +109,26 @@
   </si>
   <si>
     <t>.Cadastramento e tipificaçao de vaga</t>
+  </si>
+  <si>
+    <t>.Integração com sistema da polícia sobre carros roubados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,8 +154,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,152 +471,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CD8592-6EB6-4B54-8F7E-C6467C02028C}">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>